<commit_message>
export Execl set width height
</commit_message>
<xml_diff>
--- a/MiSA.Fresher.Amis.Core/ExcelTemplate/Danh_sach_nhan_vien.xlsx
+++ b/MiSA.Fresher.Amis.Core/ExcelTemplate/Danh_sach_nhan_vien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUE\BEAmis\BaseApiAmis\MiSA.Fresher.Amis.Core\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CDD5C1-EAC9-439D-8404-682FB26C306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21619612-272D-4228-BD41-414AD3F8A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -134,6 +134,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -455,13 +461,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC39C3C-2C18-4034-8AD0-AEBC5A6932EA}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
@@ -473,31 +479,31 @@
     <col min="9" max="9" width="26.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -526,6 +532,413 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>

</xml_diff>